<commit_message>
Add ucdb for the plan
</commit_message>
<xml_diff>
--- a/Verification_Plan.xlsx
+++ b/Verification_Plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cruial\ITI\verification\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cruial\ITI\verification\uvm\try_nd_error\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="198">
   <si>
     <t>Section</t>
   </si>
@@ -439,12 +439,6 @@
   </si>
   <si>
     <t>3.3.1</t>
-  </si>
-  <si>
-    <t>5.1</t>
-  </si>
-  <si>
-    <t>5.2</t>
   </si>
   <si>
     <t>12</t>
@@ -505,6 +499,138 @@
 * all inputs of in_a and in_b are 1's
 * inputs of in_a but in_b shouldn't be 0's ever
 * one of them is 1</t>
+  </si>
+  <si>
+    <t>fcoverage:alu_out_reseted ;</t>
+  </si>
+  <si>
+    <t>fcoverage:operation_a_and ;</t>
+  </si>
+  <si>
+    <t>fcoverage:operation_a_nand;</t>
+  </si>
+  <si>
+    <t>fcoverage:operation_b_xnor;</t>
+  </si>
+  <si>
+    <t>fcoverage:operation_a_or;</t>
+  </si>
+  <si>
+    <t>fcoverage:operation_b_or;</t>
+  </si>
+  <si>
+    <t>fcoverage:operation_a_xor;</t>
+  </si>
+  <si>
+    <t>fcoverage:operation_b_and;</t>
+  </si>
+  <si>
+    <t>fcoverage:operation_b_nor;</t>
+  </si>
+  <si>
+    <t>fcoverage:illegal_in_b_AND;</t>
+  </si>
+  <si>
+    <t>fcoverage:illegal_in_b_NAND;</t>
+  </si>
+  <si>
+    <t>fcoverage:illegal_in_b;</t>
+  </si>
+  <si>
+    <t>fcoverage:illegal_in_a;</t>
+  </si>
+  <si>
+    <t>fcoverage:alu_irq_clr;</t>
+  </si>
+  <si>
+    <t>fcoverage:all_enables_high;</t>
+  </si>
+  <si>
+    <t>4.6</t>
+  </si>
+  <si>
+    <t>5.3</t>
+  </si>
+  <si>
+    <t>4.1.1</t>
+  </si>
+  <si>
+    <t>4.1.2</t>
+  </si>
+  <si>
+    <t>4.1.3</t>
+  </si>
+  <si>
+    <t>4.1.4</t>
+  </si>
+  <si>
+    <t>4.2.1</t>
+  </si>
+  <si>
+    <t>4.2.2</t>
+  </si>
+  <si>
+    <t>4.2.3</t>
+  </si>
+  <si>
+    <t>4.2.4</t>
+  </si>
+  <si>
+    <t>4.6.1</t>
+  </si>
+  <si>
+    <t>4.7</t>
+  </si>
+  <si>
+    <t>5.4</t>
+  </si>
+  <si>
+    <t>irq_operation_a</t>
+  </si>
+  <si>
+    <t>irq_active_and</t>
+  </si>
+  <si>
+    <t>fcoverage:irq_active_and;</t>
+  </si>
+  <si>
+    <t>irq_active_nand</t>
+  </si>
+  <si>
+    <t>fcoverage:irq_active_nand;</t>
+  </si>
+  <si>
+    <t>irq_active_or</t>
+  </si>
+  <si>
+    <t>fcoverage:irq_active_or;</t>
+  </si>
+  <si>
+    <t>irq_active_xor</t>
+  </si>
+  <si>
+    <t>fcoverage:irq_active_xor;</t>
+  </si>
+  <si>
+    <t>irq_operation_b</t>
+  </si>
+  <si>
+    <t>irq_active_xnor</t>
+  </si>
+  <si>
+    <t>fcoverage:irq_active_xnor;</t>
+  </si>
+  <si>
+    <t>irq_active_nor</t>
+  </si>
+  <si>
+    <t>fcoverage:irq_active_nor;</t>
+  </si>
+  <si>
+    <t>fcoverage:op_a;</t>
+  </si>
+  <si>
+    <t>fcoverage:op_b;</t>
   </si>
 </sst>
 </file>
@@ -691,7 +817,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -753,15 +879,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="3" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -771,7 +888,28 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="3" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1108,12 +1246,12 @@
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
       <c r="D1" s="12"/>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="26"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="23"/>
       <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -1919,7 +2057,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2016,25 +2154,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="D22" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="96.77734375" customWidth="1"/>
-    <col min="4" max="4" width="42.77734375" customWidth="1"/>
-    <col min="5" max="5" width="33.44140625" customWidth="1"/>
-    <col min="6" max="6" width="39.6640625" customWidth="1"/>
-    <col min="7" max="7" width="37.33203125" customWidth="1"/>
-    <col min="8" max="8" width="12.109375" customWidth="1"/>
+    <col min="1" max="1" width="7.5546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="105.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.77734375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="41.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -2045,22 +2184,25 @@
         <v>2</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F1" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="H1" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="20">
         <v>1</v>
       </c>
@@ -2071,20 +2213,23 @@
         <v>133</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="H2" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="I2" s="18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="20">
         <v>1.1000000000000001</v>
       </c>
@@ -2094,21 +2239,22 @@
       <c r="C3" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>89</v>
-      </c>
+      <c r="D3" s="6"/>
       <c r="E3" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="H3" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="I3" s="18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="20">
         <v>2.1</v>
       </c>
@@ -2119,40 +2265,46 @@
         <v>71</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="26" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>128</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E5" s="4"/>
+        <v>163</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="F5" s="6"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="6"/>
+      <c r="I5" s="18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="20">
         <v>2.2000000000000002</v>
       </c>
@@ -2163,18 +2315,21 @@
         <v>72</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>89</v>
+        <v>156</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="F6" s="6"/>
+      <c r="F6" s="6" t="s">
+        <v>89</v>
+      </c>
       <c r="G6" s="4"/>
-      <c r="H6" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H6" s="6"/>
+      <c r="I6" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>63</v>
       </c>
@@ -2185,16 +2340,19 @@
         <v>129</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E7" s="4"/>
+        <v>164</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="F7" s="6"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="6"/>
+      <c r="I7" s="18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="20">
         <v>2.2999999999999998</v>
       </c>
@@ -2205,18 +2363,21 @@
         <v>73</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>89</v>
+        <v>158</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="F8" s="6"/>
+      <c r="F8" s="6" t="s">
+        <v>89</v>
+      </c>
       <c r="G8" s="4"/>
-      <c r="H8" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H8" s="6"/>
+      <c r="I8" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="20">
         <v>2.4</v>
       </c>
@@ -2227,18 +2388,21 @@
         <v>74</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>89</v>
+        <v>160</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="F9" s="6"/>
+      <c r="F9" s="6" t="s">
+        <v>89</v>
+      </c>
       <c r="G9" s="4"/>
-      <c r="H9" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H9" s="6"/>
+      <c r="I9" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="20">
         <v>3.1</v>
       </c>
@@ -2249,18 +2413,21 @@
         <v>76</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>89</v>
+        <v>157</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="F10" s="6"/>
+      <c r="F10" s="6" t="s">
+        <v>89</v>
+      </c>
       <c r="G10" s="4"/>
-      <c r="H10" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H10" s="6"/>
+      <c r="I10" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="20">
         <v>3.2</v>
       </c>
@@ -2271,18 +2438,21 @@
         <v>79</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>89</v>
+        <v>161</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="F11" s="6"/>
+      <c r="F11" s="6" t="s">
+        <v>89</v>
+      </c>
       <c r="G11" s="4"/>
-      <c r="H11" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H11" s="6"/>
+      <c r="I11" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>135</v>
       </c>
@@ -2293,18 +2463,21 @@
         <v>130</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E12" s="4"/>
+        <v>165</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="F12" s="6"/>
-      <c r="G12" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="H12" s="3" t="s">
+      <c r="G12" s="4"/>
+      <c r="H12" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="I12" s="18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="20">
         <v>3.3</v>
       </c>
@@ -2315,18 +2488,21 @@
         <v>78</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>89</v>
+        <v>162</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="F13" s="6"/>
+      <c r="F13" s="6" t="s">
+        <v>89</v>
+      </c>
       <c r="G13" s="4"/>
-      <c r="H13" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H13" s="6"/>
+      <c r="I13" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
         <v>136</v>
       </c>
@@ -2337,16 +2513,19 @@
         <v>80</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E14" s="4"/>
+        <v>166</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="F14" s="6"/>
       <c r="G14" s="4"/>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="6"/>
+      <c r="I14" s="18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="20">
         <v>3.4</v>
       </c>
@@ -2357,18 +2536,21 @@
         <v>81</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>89</v>
+        <v>159</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="F15" s="6"/>
+      <c r="F15" s="6" t="s">
+        <v>89</v>
+      </c>
       <c r="G15" s="4"/>
-      <c r="H15" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H15" s="6"/>
+      <c r="I15" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
         <v>99</v>
       </c>
@@ -2380,355 +2562,545 @@
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="4"/>
-      <c r="F16" s="6" t="s">
-        <v>89</v>
-      </c>
+      <c r="F16" s="6"/>
       <c r="G16" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="I16" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>100</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C17" s="29"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="31"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C18" s="29"/>
+      <c r="D18" s="30" t="s">
+        <v>184</v>
+      </c>
+      <c r="E18" s="29"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="31"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C19" s="29"/>
+      <c r="D19" s="30" t="s">
+        <v>186</v>
+      </c>
+      <c r="E19" s="29"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="31"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C20" s="29"/>
+      <c r="D20" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="E20" s="29"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="31"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C21" s="29"/>
+      <c r="D21" s="30" t="s">
+        <v>190</v>
+      </c>
+      <c r="E21" s="29"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="31"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C22" s="29"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="31"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C23" s="29"/>
+      <c r="D23" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="E23" s="29"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="31"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C24" s="29"/>
+      <c r="D24" s="30" t="s">
+        <v>184</v>
+      </c>
+      <c r="E24" s="29"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="31"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C25" s="29"/>
+      <c r="D25" s="30" t="s">
+        <v>195</v>
+      </c>
+      <c r="E25" s="29"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="31"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C26" s="29"/>
+      <c r="D26" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="E26" s="29"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="31"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="G17" s="4"/>
-      <c r="H17" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="G19" s="4"/>
-      <c r="H19" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="G20" s="4"/>
-      <c r="H20" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="G21" s="4"/>
-      <c r="H21" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="23" t="s">
-        <v>137</v>
-      </c>
-      <c r="B23" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="F23" s="6"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="20" t="s">
-        <v>138</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="20">
-        <v>6</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="20">
-        <v>7</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="G26" s="4"/>
-      <c r="H26" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="20">
-        <v>8</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="4"/>
-      <c r="F27" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="G27" s="4"/>
-      <c r="H27" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F27" s="6"/>
+      <c r="G27" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H27" s="6"/>
+      <c r="I27" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="20" t="s">
-        <v>38</v>
+        <v>103</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>89</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="D28" s="6"/>
+      <c r="E28" s="4"/>
       <c r="F28" s="6"/>
       <c r="G28" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="H28" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H28" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="I28" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
-        <v>41</v>
+        <v>106</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>111</v>
+        <v>50</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>89</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="D29" s="6"/>
+      <c r="E29" s="4"/>
       <c r="F29" s="6"/>
       <c r="G29" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="H29" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H29" s="6"/>
+      <c r="I29" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="20" t="s">
-        <v>42</v>
+        <v>169</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>151</v>
+        <v>167</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>89</v>
       </c>
       <c r="F30" s="6"/>
       <c r="G30" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+      <c r="H30" s="6"/>
+      <c r="I30" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="20" t="s">
-        <v>139</v>
+        <v>179</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>89</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="D31" s="6"/>
+      <c r="E31" s="4"/>
       <c r="F31" s="6"/>
       <c r="G31" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H31" s="6"/>
+      <c r="I31" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D32" s="6"/>
+      <c r="E32" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="F32" s="6"/>
+      <c r="G32" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="I32" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="B33" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D33" s="6"/>
+      <c r="E33" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="G33" s="4"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="I34" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="20">
+        <v>6</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="6"/>
+      <c r="E35" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="I35" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="20">
+        <v>7</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" s="6"/>
+      <c r="E36" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H36" s="6"/>
+      <c r="I36" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="20">
+        <v>8</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" s="6"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H37" s="6"/>
+      <c r="I37" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D38" s="6"/>
+      <c r="E38" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="G38" s="4"/>
+      <c r="H38" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="I38" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D39" s="6"/>
+      <c r="E39" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="G39" s="4"/>
+      <c r="H39" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="I39" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="G40" s="4"/>
+      <c r="H40" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="H31" s="3" t="s">
+      <c r="I40" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="G41" s="4"/>
+      <c r="H41" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="I41" s="18" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>